<commit_message>
comparison Gigas vs COLT virtual DC
</commit_message>
<xml_diff>
--- a/refs/calculo proveedores cloud.xlsx
+++ b/refs/calculo proveedores cloud.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="-90" windowWidth="15345" windowHeight="12075" activeTab="6"/>
@@ -13,13 +13,13 @@
     <sheet name="prov.spain" sheetId="3" r:id="rId4"/>
     <sheet name="desglose costes" sheetId="6" r:id="rId5"/>
     <sheet name="Hoja3" sheetId="11" r:id="rId6"/>
-    <sheet name="Hoja1" sheetId="12" r:id="rId7"/>
+    <sheet name="COLT vs Gigas" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Hoja3!$A$1:$L$1427</definedName>
     <definedName name="iaaspricing" localSheetId="5">Hoja3!$A$1:$I$1427</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -492,6 +492,41 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>fortu</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>fortu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sin IVA
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="iaaspricing" type="6" refreshedVersion="3" background="1" saveData="1">
@@ -513,7 +548,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10246" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10303" uniqueCount="295">
   <si>
     <t>region</t>
   </si>
@@ -1412,12 +1447,64 @@
   <si>
     <t>DC 96 gigas</t>
   </si>
+  <si>
+    <t>COLT</t>
+  </si>
+  <si>
+    <t>vCloud</t>
+  </si>
+  <si>
+    <t>COLT Essentials 8-8</t>
+  </si>
+  <si>
+    <t>COLT Enterprise 8-8</t>
+  </si>
+  <si>
+    <t>8GHz 8GB</t>
+  </si>
+  <si>
+    <t>Ratio GB/GHz</t>
+  </si>
+  <si>
+    <t>overprice</t>
+  </si>
+  <si>
+    <t>Gigas
+€/mes</t>
+  </si>
+  <si>
+    <t>#vm</t>
+  </si>
+  <si>
+    <t>Gigas
+€/vm.mes</t>
+  </si>
+  <si>
+    <t>COLT Ent
+€/vm.mes</t>
+  </si>
+  <si>
+    <t>COLT Ent
+€/mes</t>
+  </si>
+  <si>
+    <t>COLT Ess
+€/mes</t>
+  </si>
+  <si>
+    <t>COLT Ess
+€/vm.mes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1473,8 +1560,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1484,6 +1578,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1501,7 +1613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1529,6 +1641,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1623,6 +1762,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1657,6 +1797,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1832,7 +1973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2062,7 +2203,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2309,17 +2450,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K15"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.42578125" style="6" customWidth="1"/>
@@ -3811,6 +3952,46 @@
       </c>
       <c r="N47"/>
     </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E48" s="5">
+        <v>8</v>
+      </c>
+      <c r="H48" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E49" s="5">
+        <v>8</v>
+      </c>
+      <c r="H49" s="5">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3819,12 +4000,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5217,7 +5398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5409,7 +5590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1427"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -61137,15 +61318,754 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="N2"/>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <f>MIN(I3/2,J3/4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="27">
+        <v>59</v>
+      </c>
+      <c r="H3" s="27">
+        <f>G3/D3</f>
+        <v>118</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8.4</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>500</v>
+      </c>
+      <c r="M3" s="25">
+        <f>I3*15+J3*15+K3*0.1</f>
+        <v>146</v>
+      </c>
+      <c r="N3" s="18">
+        <f>(M3-G3)/G3</f>
+        <v>1.4745762711864407</v>
+      </c>
+      <c r="O3" s="25">
+        <f>M3/D3</f>
+        <v>292</v>
+      </c>
+      <c r="P3" s="23">
+        <f>I3*15+J3*8.5+K3*0.1</f>
+        <v>91.4</v>
+      </c>
+      <c r="Q3" s="20">
+        <f>(M3-P3)/G3</f>
+        <v>0.92542372881355928</v>
+      </c>
+      <c r="R3" s="23">
+        <f>P3/D3</f>
+        <v>182.8</v>
+      </c>
+      <c r="S3" s="15">
+        <f>J3/I3</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D12" si="0">MIN(I4/2,J4/4)</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="27">
+        <v>99</v>
+      </c>
+      <c r="H4" s="27">
+        <f t="shared" ref="H4:H12" si="1">G4/D4</f>
+        <v>99</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>16.8</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>750</v>
+      </c>
+      <c r="M4" s="25">
+        <f t="shared" ref="M4:M12" si="2">I4*15+J4*15+K4*0.1</f>
+        <v>292</v>
+      </c>
+      <c r="N4" s="18">
+        <f>(M4-G4)/G4</f>
+        <v>1.9494949494949494</v>
+      </c>
+      <c r="O4" s="25">
+        <f t="shared" ref="O4:O12" si="3">M4/D4</f>
+        <v>292</v>
+      </c>
+      <c r="P4" s="23">
+        <f>I4*15+J4*8.5+K4*0.1</f>
+        <v>182.8</v>
+      </c>
+      <c r="Q4" s="20">
+        <f t="shared" ref="Q4:Q12" si="4">(M4-P4)/G4</f>
+        <v>1.1030303030303028</v>
+      </c>
+      <c r="R4" s="23">
+        <f t="shared" ref="R4:R12" si="5">P4/D4</f>
+        <v>182.8</v>
+      </c>
+      <c r="S4" s="15">
+        <f t="shared" ref="S4:S12" si="6">J4/I4</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="27">
+        <v>179</v>
+      </c>
+      <c r="H5" s="27">
+        <f t="shared" si="1"/>
+        <v>89.5</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>25.2</v>
+      </c>
+      <c r="K5">
+        <v>150</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="25">
+        <f t="shared" si="2"/>
+        <v>453</v>
+      </c>
+      <c r="N5" s="18">
+        <f>(M5-G5)/G5</f>
+        <v>1.5307262569832403</v>
+      </c>
+      <c r="O5" s="25">
+        <f t="shared" si="3"/>
+        <v>226.5</v>
+      </c>
+      <c r="P5" s="23">
+        <f>I5*15+J5*8.5+K5*0.1</f>
+        <v>289.2</v>
+      </c>
+      <c r="Q5" s="20">
+        <f t="shared" si="4"/>
+        <v>0.91508379888268165</v>
+      </c>
+      <c r="R5" s="23">
+        <f t="shared" si="5"/>
+        <v>144.6</v>
+      </c>
+      <c r="S5" s="15">
+        <f t="shared" si="6"/>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="G6" s="27">
+        <v>259</v>
+      </c>
+      <c r="H6" s="27">
+        <f t="shared" si="1"/>
+        <v>86.333333333333329</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>33.6</v>
+      </c>
+      <c r="K6">
+        <v>200</v>
+      </c>
+      <c r="L6">
+        <v>1500</v>
+      </c>
+      <c r="M6" s="25">
+        <f t="shared" si="2"/>
+        <v>614</v>
+      </c>
+      <c r="N6" s="18">
+        <f>(M6-G6)/G6</f>
+        <v>1.3706563706563706</v>
+      </c>
+      <c r="O6" s="25">
+        <f t="shared" si="3"/>
+        <v>204.66666666666666</v>
+      </c>
+      <c r="P6" s="23">
+        <f>I6*15+J6*8.5+K6*0.1</f>
+        <v>395.6</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="4"/>
+        <v>0.84324324324324318</v>
+      </c>
+      <c r="R6" s="23">
+        <f t="shared" si="5"/>
+        <v>131.86666666666667</v>
+      </c>
+      <c r="S6" s="15">
+        <f t="shared" si="6"/>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="G7" s="27">
+        <v>349</v>
+      </c>
+      <c r="H7" s="27">
+        <f t="shared" si="1"/>
+        <v>87.25</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>42</v>
+      </c>
+      <c r="K7">
+        <v>250</v>
+      </c>
+      <c r="L7">
+        <v>2000</v>
+      </c>
+      <c r="M7" s="25">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+      <c r="N7" s="18">
+        <f>(M7-G7)/G7</f>
+        <v>1.2206303724928367</v>
+      </c>
+      <c r="O7" s="25">
+        <f t="shared" si="3"/>
+        <v>193.75</v>
+      </c>
+      <c r="P7" s="23">
+        <f>I7*15+J7*8.5+K7*0.1</f>
+        <v>502</v>
+      </c>
+      <c r="Q7" s="20">
+        <f t="shared" si="4"/>
+        <v>0.7822349570200573</v>
+      </c>
+      <c r="R7" s="23">
+        <f t="shared" si="5"/>
+        <v>125.5</v>
+      </c>
+      <c r="S7" s="15">
+        <f t="shared" si="6"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="G8" s="27">
+        <v>499</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="1"/>
+        <v>83.166666666666671</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>50.4</v>
+      </c>
+      <c r="K8">
+        <v>350</v>
+      </c>
+      <c r="L8">
+        <v>2500</v>
+      </c>
+      <c r="M8" s="25">
+        <f t="shared" si="2"/>
+        <v>971</v>
+      </c>
+      <c r="N8" s="18">
+        <f>(M8-G8)/G8</f>
+        <v>0.94589178356713421</v>
+      </c>
+      <c r="O8" s="25">
+        <f t="shared" si="3"/>
+        <v>161.83333333333334</v>
+      </c>
+      <c r="P8" s="23">
+        <f>I8*15+J8*8.5+K8*0.1</f>
+        <v>643.4</v>
+      </c>
+      <c r="Q8" s="20">
+        <f t="shared" si="4"/>
+        <v>0.65651302605210426</v>
+      </c>
+      <c r="R8" s="23">
+        <f t="shared" si="5"/>
+        <v>107.23333333333333</v>
+      </c>
+      <c r="S8" s="14">
+        <f t="shared" si="6"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="G9" s="27">
+        <v>649</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="1"/>
+        <v>81.125</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>63</v>
+      </c>
+      <c r="K9">
+        <v>500</v>
+      </c>
+      <c r="L9">
+        <v>3000</v>
+      </c>
+      <c r="M9" s="25">
+        <f t="shared" si="2"/>
+        <v>1235</v>
+      </c>
+      <c r="N9" s="18">
+        <f>(M9-G9)/G9</f>
+        <v>0.90292758089368264</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="3"/>
+        <v>154.375</v>
+      </c>
+      <c r="P9" s="23">
+        <f>I9*15+J9*8.5+K9*0.1</f>
+        <v>825.5</v>
+      </c>
+      <c r="Q9" s="20">
+        <f t="shared" si="4"/>
+        <v>0.63097072419106315</v>
+      </c>
+      <c r="R9" s="23">
+        <f t="shared" si="5"/>
+        <v>103.1875</v>
+      </c>
+      <c r="S9" s="14">
+        <f t="shared" si="6"/>
+        <v>3.9375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="G10" s="27">
+        <v>1099</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="1"/>
+        <v>68.6875</v>
+      </c>
+      <c r="I10">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="K10">
+        <v>600</v>
+      </c>
+      <c r="L10">
+        <v>3500</v>
+      </c>
+      <c r="M10" s="25">
+        <f t="shared" si="2"/>
+        <v>1674</v>
+      </c>
+      <c r="N10" s="18">
+        <f>(M10-G10)/G10</f>
+        <v>0.52320291173794353</v>
+      </c>
+      <c r="O10" s="25">
+        <f t="shared" si="3"/>
+        <v>104.625</v>
+      </c>
+      <c r="P10" s="23">
+        <f>I10*15+J10*8.5+K10*0.1</f>
+        <v>1182.5999999999999</v>
+      </c>
+      <c r="Q10" s="20">
+        <f t="shared" si="4"/>
+        <v>0.44713375796178351</v>
+      </c>
+      <c r="R10" s="23">
+        <f t="shared" si="5"/>
+        <v>73.912499999999994</v>
+      </c>
+      <c r="S10" s="14">
+        <f t="shared" si="6"/>
+        <v>2.3624999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>22.05</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="G11" s="27">
+        <v>1899</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="1"/>
+        <v>86.122448979591837</v>
+      </c>
+      <c r="I11">
+        <v>64</v>
+      </c>
+      <c r="J11">
+        <v>88.2</v>
+      </c>
+      <c r="K11">
+        <v>700</v>
+      </c>
+      <c r="L11">
+        <v>4000</v>
+      </c>
+      <c r="M11" s="25">
+        <f t="shared" si="2"/>
+        <v>2353</v>
+      </c>
+      <c r="N11" s="18">
+        <f>(M11-G11)/G11</f>
+        <v>0.23907319641916799</v>
+      </c>
+      <c r="O11" s="25">
+        <f t="shared" si="3"/>
+        <v>106.71201814058956</v>
+      </c>
+      <c r="P11" s="23">
+        <f>I11*15+J11*8.5+K11*0.1</f>
+        <v>1779.7</v>
+      </c>
+      <c r="Q11" s="20">
+        <f t="shared" si="4"/>
+        <v>0.30189573459715635</v>
+      </c>
+      <c r="R11" s="23">
+        <f t="shared" si="5"/>
+        <v>80.712018140589564</v>
+      </c>
+      <c r="S11" s="14">
+        <f t="shared" si="6"/>
+        <v>1.378125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>96</v>
+      </c>
+      <c r="G12" s="27">
+        <v>2499</v>
+      </c>
+      <c r="H12" s="27">
+        <f t="shared" si="1"/>
+        <v>99.96</v>
+      </c>
+      <c r="I12">
+        <v>96</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>5000</v>
+      </c>
+      <c r="M12" s="25">
+        <f t="shared" si="2"/>
+        <v>3040</v>
+      </c>
+      <c r="N12" s="18">
+        <f>(M12-G12)/G12</f>
+        <v>0.21648659463785513</v>
+      </c>
+      <c r="O12" s="25">
+        <f t="shared" si="3"/>
+        <v>121.6</v>
+      </c>
+      <c r="P12" s="23">
+        <f>I12*15+J12*8.5+K12*0.1</f>
+        <v>2390</v>
+      </c>
+      <c r="Q12" s="20">
+        <f>(M12-P12)/G12</f>
+        <v>0.26010404161664669</v>
+      </c>
+      <c r="R12" s="23">
+        <f t="shared" si="5"/>
+        <v>95.6</v>
+      </c>
+      <c r="S12" s="14">
+        <f t="shared" si="6"/>
+        <v>1.0416666666666667</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>